<commit_message>
Thêm update database version
</commit_message>
<xml_diff>
--- a/BiTech.Library/BiTech.Library/Tempalates/MauSach.xlsx
+++ b/BiTech.Library/BiTech.Library/Tempalates/MauSach.xlsx
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -640,6 +640,7 @@
     <col min="15" max="15" width="33" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">

</xml_diff>